<commit_message>
trabajo del 05 agosto 2020
</commit_message>
<xml_diff>
--- a/GompertzCol.xlsx
+++ b/GompertzCol.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>4.152910151788866e-06</v>
+        <v>2.98526176267766e-06</v>
       </c>
     </row>
     <row r="4">
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="n">
-        <v>4.152910151788866e-06</v>
+        <v>2.98526176267766e-06</v>
       </c>
     </row>
     <row r="5">
@@ -492,7 +492,7 @@
         <v>4</v>
       </c>
       <c r="H5" t="n">
-        <v>4.152910151788866e-06</v>
+        <v>2.98526176267766e-06</v>
       </c>
     </row>
     <row r="6">
@@ -514,7 +514,7 @@
         <v>5</v>
       </c>
       <c r="H6" t="n">
-        <v>8.305820303577732e-06</v>
+        <v>5.970523525355321e-06</v>
       </c>
     </row>
     <row r="7">
@@ -536,7 +536,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="n">
-        <v>1.24587304553666e-05</v>
+        <v>8.955785288032982e-06</v>
       </c>
     </row>
     <row r="8">
@@ -558,7 +558,7 @@
         <v>7</v>
       </c>
       <c r="H8" t="n">
-        <v>2.076455075894433e-05</v>
+        <v>1.49263088133883e-05</v>
       </c>
     </row>
     <row r="9">
@@ -580,7 +580,7 @@
         <v>8</v>
       </c>
       <c r="H9" t="n">
-        <v>3.322328121431093e-05</v>
+        <v>2.388209410142128e-05</v>
       </c>
     </row>
     <row r="10">
@@ -602,7 +602,7 @@
         <v>9</v>
       </c>
       <c r="H10" t="n">
-        <v>4.983492182146639e-05</v>
+        <v>3.582314115213193e-05</v>
       </c>
     </row>
     <row r="11">
@@ -624,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="H11" t="n">
-        <v>8.305820303577732e-05</v>
+        <v>5.970523525355321e-05</v>
       </c>
     </row>
     <row r="12">
@@ -646,7 +646,7 @@
         <v>11</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0001287402147054548</v>
+        <v>9.254311464300747e-05</v>
       </c>
     </row>
     <row r="13">
@@ -668,7 +668,7 @@
         <v>12</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0001827280466787101</v>
+        <v>0.0001313515175578171</v>
       </c>
     </row>
     <row r="14">
@@ -690,7 +690,7 @@
         <v>13</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0002657862497144874</v>
+        <v>0.0001910567528113703</v>
       </c>
     </row>
     <row r="15">
@@ -712,7 +712,7 @@
         <v>14</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0003446915425984759</v>
+        <v>0.0002477767263022458</v>
       </c>
     </row>
     <row r="16">
@@ -734,7 +734,7 @@
         <v>15</v>
       </c>
       <c r="H16" t="n">
-        <v>0.000465125937000353</v>
+        <v>0.000334349317419898</v>
       </c>
     </row>
     <row r="17">
@@ -756,7 +756,7 @@
         <v>16</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0006395481633754853</v>
+        <v>0.0004597303114523597</v>
       </c>
     </row>
     <row r="18">
@@ -778,7 +778,7 @@
         <v>17</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0008222762100541954</v>
+        <v>0.0005910818290101767</v>
       </c>
     </row>
     <row r="19">
@@ -800,7 +800,7 @@
         <v>18</v>
       </c>
       <c r="H19" t="n">
-        <v>0.001108827010527627</v>
+        <v>0.0007970648906349354</v>
       </c>
     </row>
     <row r="20">
@@ -822,7 +822,7 @@
         <v>19</v>
       </c>
       <c r="H20" t="n">
-        <v>0.001432754002367159</v>
+        <v>0.001029915308123793</v>
       </c>
     </row>
     <row r="21">
@@ -844,7 +844,7 @@
         <v>20</v>
       </c>
       <c r="H21" t="n">
-        <v>0.001764986814510268</v>
+        <v>0.001268736249138006</v>
       </c>
     </row>
     <row r="22">
@@ -866,7 +866,7 @@
         <v>21</v>
       </c>
       <c r="H22" t="n">
-        <v>0.002105525446956955</v>
+        <v>0.001513527713677574</v>
       </c>
     </row>
     <row r="23">
@@ -888,7 +888,7 @@
         <v>22</v>
       </c>
       <c r="H23" t="n">
-        <v>0.002495899001225108</v>
+        <v>0.001794142319369274</v>
       </c>
     </row>
     <row r="24">
@@ -910,7 +910,7 @@
         <v>23</v>
       </c>
       <c r="H24" t="n">
-        <v>0.003081459332627339</v>
+        <v>0.002215064227906824</v>
       </c>
     </row>
     <row r="25">
@@ -932,7 +932,7 @@
         <v>24</v>
       </c>
       <c r="H25" t="n">
-        <v>0.003758383687368924</v>
+        <v>0.002701661895223283</v>
       </c>
     </row>
     <row r="26">
@@ -954,7 +954,7 @@
         <v>25</v>
       </c>
       <c r="H26" t="n">
-        <v>0.004418696401503354</v>
+        <v>0.003176318515489031</v>
       </c>
     </row>
     <row r="27">
@@ -976,7 +976,7 @@
         <v>26</v>
       </c>
       <c r="H27" t="n">
-        <v>0.005083162025789572</v>
+        <v>0.003653960397517456</v>
       </c>
     </row>
     <row r="28">
@@ -998,7 +998,7 @@
         <v>27</v>
       </c>
       <c r="H28" t="n">
-        <v>0.005772545110986523</v>
+        <v>0.004149513850121948</v>
       </c>
     </row>
     <row r="29">
@@ -1020,7 +1020,7 @@
         <v>28</v>
       </c>
       <c r="H29" t="n">
-        <v>0.006345646711933387</v>
+        <v>0.004561479973371465</v>
       </c>
     </row>
     <row r="30">
@@ -1042,7 +1042,7 @@
         <v>29</v>
       </c>
       <c r="H30" t="n">
-        <v>0.007151311281380427</v>
+        <v>0.005140620755330931</v>
       </c>
     </row>
     <row r="31">
@@ -1064,7 +1064,7 @@
         <v>30</v>
       </c>
       <c r="H31" t="n">
-        <v>0.007940364210220312</v>
+        <v>0.005707820490239686</v>
       </c>
     </row>
     <row r="32">
@@ -1086,7 +1086,7 @@
         <v>31</v>
       </c>
       <c r="H32" t="n">
-        <v>0.00875018168981914</v>
+        <v>0.006289946533961831</v>
       </c>
     </row>
     <row r="33">
@@ -1108,7 +1108,7 @@
         <v>32</v>
       </c>
       <c r="H33" t="n">
-        <v>0.009439564775016092</v>
+        <v>0.006785499986566322</v>
       </c>
     </row>
     <row r="34">
@@ -1130,7 +1130,7 @@
         <v>33</v>
       </c>
       <c r="H34" t="n">
-        <v>0.01021615897340061</v>
+        <v>0.007343743936187044</v>
       </c>
     </row>
     <row r="35">
@@ -1152,7 +1152,7 @@
         <v>34</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01088062459768683</v>
+        <v>0.007821385818215469</v>
       </c>
     </row>
     <row r="36">
@@ -1174,7 +1174,7 @@
         <v>35</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0113000685230175</v>
+        <v>0.008122897256245914</v>
       </c>
     </row>
     <row r="37">
@@ -1196,7 +1196,7 @@
         <v>36</v>
       </c>
       <c r="H37" t="n">
-        <v>0.01192300504578583</v>
+        <v>0.008570686520647562</v>
       </c>
     </row>
     <row r="38">
@@ -1218,7 +1218,7 @@
         <v>37</v>
       </c>
       <c r="H38" t="n">
-        <v>0.01257501193961669</v>
+        <v>0.009039372617387955</v>
       </c>
     </row>
     <row r="39">
@@ -1240,7 +1240,7 @@
         <v>38</v>
       </c>
       <c r="H39" t="n">
-        <v>0.01309827861874208</v>
+        <v>0.009415515599485341</v>
       </c>
     </row>
     <row r="40">
@@ -1256,13 +1256,13 @@
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="n">
-        <v>3295</v>
+        <v>3296</v>
       </c>
       <c r="G40" t="n">
         <v>39</v>
       </c>
       <c r="H40" t="n">
-        <v>0.01368383895014431</v>
+        <v>0.009839422769785569</v>
       </c>
     </row>
     <row r="41">
@@ -1278,13 +1278,13 @@
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
-        <v>3416</v>
+        <v>3417</v>
       </c>
       <c r="G41" t="n">
         <v>40</v>
       </c>
       <c r="H41" t="n">
-        <v>0.01418634107851077</v>
+        <v>0.01020063944306957</v>
       </c>
     </row>
     <row r="42">
@@ -1300,13 +1300,13 @@
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
-        <v>3664</v>
+        <v>3665</v>
       </c>
       <c r="G42" t="n">
         <v>41</v>
       </c>
       <c r="H42" t="n">
-        <v>0.01521626279615441</v>
+        <v>0.01094098436021363</v>
       </c>
     </row>
     <row r="43">
@@ -1322,13 +1322,13 @@
       <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="n">
-        <v>3821</v>
+        <v>3822</v>
       </c>
       <c r="G43" t="n">
         <v>42</v>
       </c>
       <c r="H43" t="n">
-        <v>0.01586826968998526</v>
+        <v>0.01140967045695402</v>
       </c>
     </row>
     <row r="44">
@@ -1344,13 +1344,13 @@
       <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="n">
-        <v>4007</v>
+        <v>4008</v>
       </c>
       <c r="G44" t="n">
         <v>43</v>
       </c>
       <c r="H44" t="n">
-        <v>0.01664071097821799</v>
+        <v>0.01196492914481206</v>
       </c>
     </row>
     <row r="45">
@@ -1366,13 +1366,13 @@
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="n">
-        <v>4245</v>
+        <v>4246</v>
       </c>
       <c r="G45" t="n">
         <v>44</v>
       </c>
       <c r="H45" t="n">
-        <v>0.01762910359434374</v>
+        <v>0.01267542144432935</v>
       </c>
     </row>
     <row r="46">
@@ -1388,13 +1388,13 @@
       <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="n">
-        <v>4414</v>
+        <v>4415</v>
       </c>
       <c r="G46" t="n">
         <v>45</v>
       </c>
       <c r="H46" t="n">
-        <v>0.01833094540999606</v>
+        <v>0.01317993068222187</v>
       </c>
     </row>
     <row r="47">
@@ -1410,13 +1410,13 @@
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
-        <v>4671</v>
+        <v>4672</v>
       </c>
       <c r="G47" t="n">
         <v>46</v>
       </c>
       <c r="H47" t="n">
-        <v>0.01939824331900579</v>
+        <v>0.01394714295523003</v>
       </c>
     </row>
     <row r="48">
@@ -1432,13 +1432,13 @@
       <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="n">
-        <v>4850</v>
+        <v>4851</v>
       </c>
       <c r="G48" t="n">
         <v>47</v>
       </c>
       <c r="H48" t="n">
-        <v>0.020141614236176</v>
+        <v>0.01448150481074933</v>
       </c>
     </row>
     <row r="49">
@@ -1454,13 +1454,13 @@
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="n">
-        <v>5056</v>
+        <v>5057</v>
       </c>
       <c r="G49" t="n">
         <v>48</v>
       </c>
       <c r="H49" t="n">
-        <v>0.02099711372744451</v>
+        <v>0.01509646873386093</v>
       </c>
     </row>
     <row r="50">
@@ -1476,13 +1476,13 @@
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="n">
-        <v>5277</v>
+        <v>5278</v>
       </c>
       <c r="G50" t="n">
         <v>49</v>
       </c>
       <c r="H50" t="n">
-        <v>0.02191490687098985</v>
+        <v>0.01575621158341269</v>
       </c>
     </row>
     <row r="51">
@@ -1498,13 +1498,13 @@
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="n">
-        <v>5494</v>
+        <v>5495</v>
       </c>
       <c r="G51" t="n">
         <v>50</v>
       </c>
       <c r="H51" t="n">
-        <v>0.02281608837392803</v>
+        <v>0.01640401338591374</v>
       </c>
     </row>
     <row r="52">
@@ -1520,13 +1520,13 @@
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="n">
-        <v>5715</v>
+        <v>5716</v>
       </c>
       <c r="G52" t="n">
         <v>51</v>
       </c>
       <c r="H52" t="n">
-        <v>0.02373388151747337</v>
+        <v>0.01706375623546551</v>
       </c>
     </row>
     <row r="53">
@@ -1542,13 +1542,13 @@
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="n">
-        <v>5963</v>
+        <v>5964</v>
       </c>
       <c r="G53" t="n">
         <v>52</v>
       </c>
       <c r="H53" t="n">
-        <v>0.02476380323511701</v>
+        <v>0.01780410115260957</v>
       </c>
     </row>
     <row r="54">
@@ -1564,13 +1564,13 @@
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="n">
-        <v>6265</v>
+        <v>6266</v>
       </c>
       <c r="G54" t="n">
         <v>53</v>
       </c>
       <c r="H54" t="n">
-        <v>0.02601798210095724</v>
+        <v>0.01870565020493822</v>
       </c>
     </row>
     <row r="55">
@@ -1586,13 +1586,13 @@
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="n">
-        <v>6571</v>
+        <v>6572</v>
       </c>
       <c r="G55" t="n">
         <v>54</v>
       </c>
       <c r="H55" t="n">
-        <v>0.02728877260740464</v>
+        <v>0.01961914030431759</v>
       </c>
     </row>
     <row r="56">
@@ -1608,13 +1608,13 @@
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="n">
-        <v>6877</v>
+        <v>6878</v>
       </c>
       <c r="G56" t="n">
         <v>55</v>
       </c>
       <c r="H56" t="n">
-        <v>0.02855956311385203</v>
+        <v>0.02053263040369695</v>
       </c>
     </row>
     <row r="57">
@@ -1630,13 +1630,13 @@
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="n">
-        <v>7129</v>
+        <v>7130</v>
       </c>
       <c r="G57" t="n">
         <v>56</v>
       </c>
       <c r="H57" t="n">
-        <v>0.02960609647210283</v>
+        <v>0.02128491636789172</v>
       </c>
     </row>
     <row r="58">
@@ -1652,13 +1652,13 @@
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="n">
-        <v>7537</v>
+        <v>7538</v>
       </c>
       <c r="G58" t="n">
         <v>57</v>
       </c>
       <c r="H58" t="n">
-        <v>0.03130048381403269</v>
+        <v>0.0225029031670642</v>
       </c>
     </row>
     <row r="59">
@@ -1674,13 +1674,13 @@
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="n">
-        <v>8053</v>
+        <v>8054</v>
       </c>
       <c r="G59" t="n">
         <v>58</v>
       </c>
       <c r="H59" t="n">
-        <v>0.03344338545235574</v>
+        <v>0.02404329823660588</v>
       </c>
     </row>
     <row r="60">
@@ -1696,13 +1696,13 @@
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="n">
-        <v>8431</v>
+        <v>8432</v>
       </c>
       <c r="G60" t="n">
         <v>59</v>
       </c>
       <c r="H60" t="n">
-        <v>0.03501318548973193</v>
+        <v>0.02517172718289803</v>
       </c>
     </row>
     <row r="61">
@@ -1718,13 +1718,13 @@
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="n">
-        <v>8906</v>
+        <v>8907</v>
       </c>
       <c r="G61" t="n">
         <v>60</v>
       </c>
       <c r="H61" t="n">
-        <v>0.03698581781183164</v>
+        <v>0.02658972652016992</v>
       </c>
     </row>
     <row r="62">
@@ -1740,13 +1740,13 @@
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="n">
-        <v>9371</v>
+        <v>9373</v>
       </c>
       <c r="G62" t="n">
         <v>61</v>
       </c>
       <c r="H62" t="n">
-        <v>0.03891692103241346</v>
+        <v>0.02798085850157771</v>
       </c>
     </row>
     <row r="63">
@@ -1762,13 +1762,13 @@
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="n">
-        <v>9835</v>
+        <v>9837</v>
       </c>
       <c r="G63" t="n">
         <v>62</v>
       </c>
       <c r="H63" t="n">
-        <v>0.0408438713428435</v>
+        <v>0.02936601995946015</v>
       </c>
     </row>
     <row r="64">
@@ -1784,13 +1784,13 @@
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="n">
-        <v>10227</v>
+        <v>10229</v>
       </c>
       <c r="G64" t="n">
         <v>63</v>
       </c>
       <c r="H64" t="n">
-        <v>0.04247181212234474</v>
+        <v>0.03053624257042979</v>
       </c>
     </row>
     <row r="65">
@@ -1806,13 +1806,13 @@
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="n">
-        <v>10737</v>
+        <v>10739</v>
       </c>
       <c r="G65" t="n">
         <v>64</v>
       </c>
       <c r="H65" t="n">
-        <v>0.04458979629975705</v>
+        <v>0.03205872606939539</v>
       </c>
     </row>
     <row r="66">
@@ -1828,13 +1828,13 @@
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="n">
-        <v>11525</v>
+        <v>11527</v>
       </c>
       <c r="G66" t="n">
         <v>65</v>
       </c>
       <c r="H66" t="n">
-        <v>0.04786228949936668</v>
+        <v>0.03441111233838539</v>
       </c>
     </row>
     <row r="67">
@@ -1850,13 +1850,13 @@
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="n">
-        <v>12271</v>
+        <v>12274</v>
       </c>
       <c r="G67" t="n">
         <v>66</v>
       </c>
       <c r="H67" t="n">
-        <v>0.05096036047260118</v>
+        <v>0.0366411028751056</v>
       </c>
     </row>
     <row r="68">
@@ -1872,13 +1872,13 @@
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="n">
-        <v>13041</v>
+        <v>13045</v>
       </c>
       <c r="G68" t="n">
         <v>67</v>
       </c>
       <c r="H68" t="n">
-        <v>0.0541581012894786</v>
+        <v>0.03894273969413008</v>
       </c>
     </row>
     <row r="69">
@@ -1894,13 +1894,13 @@
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="n">
-        <v>14020</v>
+        <v>14024</v>
       </c>
       <c r="G69" t="n">
         <v>68</v>
       </c>
       <c r="H69" t="n">
-        <v>0.0582238003280799</v>
+        <v>0.04186531095979151</v>
       </c>
     </row>
     <row r="70">
@@ -1916,13 +1916,13 @@
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="n">
-        <v>14763</v>
+        <v>14767</v>
       </c>
       <c r="G70" t="n">
         <v>69</v>
       </c>
       <c r="H70" t="n">
-        <v>0.06130941257085903</v>
+        <v>0.04408336044946101</v>
       </c>
     </row>
     <row r="71">
@@ -1938,13 +1938,13 @@
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="n">
-        <v>15235</v>
+        <v>15239</v>
       </c>
       <c r="G71" t="n">
         <v>70</v>
       </c>
       <c r="H71" t="n">
-        <v>0.06326958616250337</v>
+        <v>0.04549240400144487</v>
       </c>
     </row>
     <row r="72">
@@ -1960,13 +1960,13 @@
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="n">
-        <v>15966</v>
+        <v>15971</v>
       </c>
       <c r="G72" t="n">
         <v>71</v>
       </c>
       <c r="H72" t="n">
-        <v>0.06630536348346104</v>
+        <v>0.04767761561172491</v>
       </c>
     </row>
     <row r="73">
@@ -1982,13 +1982,13 @@
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="n">
-        <v>16787</v>
+        <v>16793</v>
       </c>
       <c r="G73" t="n">
         <v>72</v>
       </c>
       <c r="H73" t="n">
-        <v>0.06971490271807969</v>
+        <v>0.05013150078064595</v>
       </c>
     </row>
     <row r="74">
@@ -2004,13 +2004,13 @@
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="n">
-        <v>17634</v>
+        <v>17640</v>
       </c>
       <c r="G74" t="n">
         <v>73</v>
       </c>
       <c r="H74" t="n">
-        <v>0.07323241761664487</v>
+        <v>0.05266001749363393</v>
       </c>
     </row>
     <row r="75">
@@ -2026,13 +2026,13 @@
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="n">
-        <v>18693</v>
+        <v>18699</v>
       </c>
       <c r="G75" t="n">
         <v>74</v>
       </c>
       <c r="H75" t="n">
-        <v>0.07763034946738927</v>
+        <v>0.05582140970030957</v>
       </c>
     </row>
     <row r="76">
@@ -2048,13 +2048,13 @@
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="n">
-        <v>19668</v>
+        <v>19674</v>
       </c>
       <c r="G76" t="n">
         <v>75</v>
       </c>
       <c r="H76" t="n">
-        <v>0.08167943686538341</v>
+        <v>0.05873203991892029</v>
       </c>
     </row>
     <row r="77">
@@ -2070,13 +2070,13 @@
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="n">
-        <v>20573</v>
+        <v>20579</v>
       </c>
       <c r="G77" t="n">
         <v>76</v>
       </c>
       <c r="H77" t="n">
-        <v>0.08543782055275234</v>
+        <v>0.06143370181414357</v>
       </c>
     </row>
     <row r="78">
@@ -2092,13 +2092,13 @@
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="n">
-        <v>21415</v>
+        <v>21421</v>
       </c>
       <c r="G78" t="n">
         <v>77</v>
       </c>
       <c r="H78" t="n">
-        <v>0.08893457090055856</v>
+        <v>0.06394729221831816</v>
       </c>
     </row>
     <row r="79">
@@ -2114,13 +2114,13 @@
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="n">
-        <v>22615</v>
+        <v>22621</v>
       </c>
       <c r="G79" t="n">
         <v>78</v>
       </c>
       <c r="H79" t="n">
-        <v>0.0939180630827052</v>
+        <v>0.06752960633353136</v>
       </c>
     </row>
     <row r="80">
@@ -2136,13 +2136,13 @@
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="n">
-        <v>23776</v>
+        <v>23782</v>
       </c>
       <c r="G80" t="n">
         <v>79</v>
       </c>
       <c r="H80" t="n">
-        <v>0.09873959176893207</v>
+        <v>0.07099549524000012</v>
       </c>
     </row>
     <row r="81">
@@ -2158,13 +2158,13 @@
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="n">
-        <v>25171</v>
+        <v>25177</v>
       </c>
       <c r="G81" t="n">
         <v>80</v>
       </c>
       <c r="H81" t="n">
-        <v>0.1045329014306775</v>
+        <v>0.07515993539893545</v>
       </c>
     </row>
     <row r="82">
@@ -2180,13 +2180,13 @@
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="n">
-        <v>26533</v>
+        <v>26540</v>
       </c>
       <c r="G82" t="n">
         <v>81</v>
       </c>
       <c r="H82" t="n">
-        <v>0.110189165057414</v>
+        <v>0.07922884718146511</v>
       </c>
     </row>
     <row r="83">
@@ -2202,13 +2202,13 @@
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="n">
-        <v>27944</v>
+        <v>27951</v>
       </c>
       <c r="G83" t="n">
         <v>82</v>
       </c>
       <c r="H83" t="n">
-        <v>0.1160489212815881</v>
+        <v>0.08344105152860329</v>
       </c>
     </row>
     <row r="84">
@@ -2224,13 +2224,13 @@
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="n">
-        <v>29365</v>
+        <v>29372</v>
       </c>
       <c r="G84" t="n">
         <v>83</v>
       </c>
       <c r="H84" t="n">
-        <v>0.1219502066072801</v>
+        <v>0.08768310849336824</v>
       </c>
     </row>
     <row r="85">
@@ -2246,13 +2246,13 @@
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="n">
-        <v>30272</v>
+        <v>30279</v>
       </c>
       <c r="G85" t="n">
         <v>84</v>
       </c>
       <c r="H85" t="n">
-        <v>0.1257168961149525</v>
+        <v>0.09039074091211688</v>
       </c>
     </row>
     <row r="86">
@@ -2268,13 +2268,13 @@
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="n">
-        <v>31429</v>
+        <v>31436</v>
       </c>
       <c r="G86" t="n">
         <v>85</v>
       </c>
       <c r="H86" t="n">
-        <v>0.1305218131605723</v>
+        <v>0.09384468877153493</v>
       </c>
     </row>
     <row r="87">
@@ -2290,13 +2290,13 @@
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="n">
-        <v>32948</v>
+        <v>32954</v>
       </c>
       <c r="G87" t="n">
         <v>86</v>
       </c>
       <c r="H87" t="n">
-        <v>0.1368300836811396</v>
+        <v>0.09837631612727962</v>
       </c>
     </row>
     <row r="88">
@@ -2312,13 +2312,13 @@
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="n">
-        <v>34317</v>
+        <v>34320</v>
       </c>
       <c r="G88" t="n">
         <v>87</v>
       </c>
       <c r="H88" t="n">
-        <v>0.1425154176789385</v>
+        <v>0.1024541836950973</v>
       </c>
     </row>
     <row r="89">
@@ -2334,13 +2334,13 @@
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="n">
-        <v>35726</v>
+        <v>35728</v>
       </c>
       <c r="G89" t="n">
         <v>88</v>
       </c>
       <c r="H89" t="n">
-        <v>0.148366868082809</v>
+        <v>0.1066574322569474</v>
       </c>
     </row>
     <row r="90">
@@ -2356,13 +2356,13 @@
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="n">
-        <v>37135</v>
+        <v>37137</v>
       </c>
       <c r="G90" t="n">
         <v>89</v>
       </c>
       <c r="H90" t="n">
-        <v>0.1542183184866796</v>
+        <v>0.1108636660805603</v>
       </c>
     </row>
     <row r="91">
@@ -2378,13 +2378,13 @@
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="n">
-        <v>38434</v>
+        <v>38436</v>
       </c>
       <c r="G91" t="n">
         <v>90</v>
       </c>
       <c r="H91" t="n">
-        <v>0.1596129487738533</v>
+        <v>0.1147415211102785</v>
       </c>
     </row>
     <row r="92">
@@ -2400,13 +2400,13 @@
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="n">
-        <v>39473</v>
+        <v>39475</v>
       </c>
       <c r="G92" t="n">
         <v>91</v>
       </c>
       <c r="H92" t="n">
-        <v>0.1639278224215619</v>
+        <v>0.1178432080817006</v>
       </c>
     </row>
     <row r="93">
@@ -2422,13 +2422,13 @@
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr"/>
       <c r="F93" t="n">
-        <v>41213</v>
+        <v>41216</v>
       </c>
       <c r="G93" t="n">
         <v>92</v>
       </c>
       <c r="H93" t="n">
-        <v>0.1711538860856745</v>
+        <v>0.1230405488105225</v>
       </c>
     </row>
     <row r="94">
@@ -2444,13 +2444,13 @@
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr"/>
       <c r="F94" t="n">
-        <v>42858</v>
+        <v>42862</v>
       </c>
       <c r="G94" t="n">
         <v>93</v>
       </c>
       <c r="H94" t="n">
-        <v>0.1779854232853672</v>
+        <v>0.1279542896718899</v>
       </c>
     </row>
     <row r="95">
@@ -2466,13 +2466,13 @@
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
       <c r="F95" t="n">
-        <v>44749</v>
+        <v>44753</v>
       </c>
       <c r="G95" t="n">
         <v>94</v>
       </c>
       <c r="H95" t="n">
-        <v>0.1858385763824</v>
+        <v>0.1335994196651133</v>
       </c>
     </row>
     <row r="96">
@@ -2488,13 +2488,13 @@
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
       <c r="F96" t="n">
-        <v>46523</v>
+        <v>46527</v>
       </c>
       <c r="G96" t="n">
         <v>95</v>
       </c>
       <c r="H96" t="n">
-        <v>0.1932058389916734</v>
+        <v>0.1388952740321035</v>
       </c>
     </row>
     <row r="97">
@@ -2510,13 +2510,13 @@
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
       <c r="F97" t="n">
-        <v>48535</v>
+        <v>48539</v>
       </c>
       <c r="G97" t="n">
         <v>96</v>
       </c>
       <c r="H97" t="n">
-        <v>0.2015614942170726</v>
+        <v>0.144901620698611</v>
       </c>
     </row>
     <row r="98">
@@ -2532,13 +2532,13 @@
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
       <c r="F98" t="n">
-        <v>50329</v>
+        <v>50336</v>
       </c>
       <c r="G98" t="n">
         <v>97</v>
       </c>
       <c r="H98" t="n">
-        <v>0.2090118150293818</v>
+        <v>0.1502661360861427</v>
       </c>
     </row>
     <row r="99">
@@ -2554,13 +2554,13 @@
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
       <c r="F99" t="n">
-        <v>51796</v>
+        <v>51803</v>
       </c>
       <c r="G99" t="n">
         <v>98</v>
       </c>
       <c r="H99" t="n">
-        <v>0.2151041342220561</v>
+        <v>0.1546455150919908</v>
       </c>
     </row>
     <row r="100">
@@ -2576,13 +2576,13 @@
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
       <c r="F100" t="n">
-        <v>54331</v>
+        <v>54338</v>
       </c>
       <c r="G100" t="n">
         <v>99</v>
       </c>
       <c r="H100" t="n">
-        <v>0.2256317614568409</v>
+        <v>0.1622131536603787</v>
       </c>
     </row>
     <row r="101">
@@ -2598,13 +2598,13 @@
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
       <c r="F101" t="n">
-        <v>56749</v>
+        <v>56760</v>
       </c>
       <c r="G101" t="n">
         <v>100</v>
       </c>
       <c r="H101" t="n">
-        <v>0.2356734982038663</v>
+        <v>0.169443457649584</v>
       </c>
     </row>
     <row r="102">
@@ -2620,13 +2620,13 @@
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
       <c r="F102" t="n">
-        <v>59536</v>
+        <v>59550</v>
       </c>
       <c r="G102" t="n">
         <v>101</v>
       </c>
       <c r="H102" t="n">
-        <v>0.2472476587969019</v>
+        <v>0.1777723379674547</v>
       </c>
     </row>
     <row r="103">
@@ -2642,13 +2642,13 @@
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
       <c r="F103" t="n">
-        <v>62483</v>
+        <v>62500</v>
       </c>
       <c r="G103" t="n">
         <v>102</v>
       </c>
       <c r="H103" t="n">
-        <v>0.2594862850142237</v>
+        <v>0.1865788601673538</v>
       </c>
     </row>
     <row r="104">
@@ -2664,13 +2664,13 @@
       <c r="D104" t="inlineStr"/>
       <c r="E104" t="inlineStr"/>
       <c r="F104" t="n">
-        <v>65431</v>
+        <v>65452</v>
       </c>
       <c r="G104" t="n">
         <v>103</v>
       </c>
       <c r="H104" t="n">
-        <v>0.2717290641416973</v>
+        <v>0.1953913528907782</v>
       </c>
     </row>
     <row r="105">
@@ -2686,13 +2686,13 @@
       <c r="D105" t="inlineStr"/>
       <c r="E105" t="inlineStr"/>
       <c r="F105" t="n">
-        <v>67892</v>
+        <v>67914</v>
       </c>
       <c r="G105" t="n">
         <v>104</v>
       </c>
       <c r="H105" t="n">
-        <v>0.2819493760252497</v>
+        <v>0.2027410673504906</v>
       </c>
     </row>
     <row r="106">
@@ -2708,13 +2708,13 @@
       <c r="D106" t="inlineStr"/>
       <c r="E106" t="inlineStr"/>
       <c r="F106" t="n">
-        <v>69540</v>
+        <v>69566</v>
       </c>
       <c r="G106" t="n">
         <v>105</v>
       </c>
       <c r="H106" t="n">
-        <v>0.2887933719553977</v>
+        <v>0.2076727197824341</v>
       </c>
     </row>
     <row r="107">
@@ -2730,13 +2730,13 @@
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="inlineStr"/>
       <c r="F107" t="n">
-        <v>71426</v>
+        <v>71452</v>
       </c>
       <c r="G107" t="n">
         <v>106</v>
       </c>
       <c r="H107" t="n">
-        <v>0.2966257605016716</v>
+        <v>0.2133029234668442</v>
       </c>
     </row>
     <row r="108">
@@ -2752,13 +2752,13 @@
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="inlineStr"/>
       <c r="F108" t="n">
-        <v>75147</v>
+        <v>75177</v>
       </c>
       <c r="G108" t="n">
         <v>107</v>
       </c>
       <c r="H108" t="n">
-        <v>0.3120787391764779</v>
+        <v>0.2244230235328185</v>
       </c>
     </row>
     <row r="109">
@@ -2774,13 +2774,13 @@
       <c r="D109" t="inlineStr"/>
       <c r="E109" t="inlineStr"/>
       <c r="F109" t="n">
-        <v>79121</v>
+        <v>79158</v>
       </c>
       <c r="G109" t="n">
         <v>108</v>
       </c>
       <c r="H109" t="n">
-        <v>0.3285824041196869</v>
+        <v>0.2363073506100382</v>
       </c>
     </row>
     <row r="110">
@@ -2796,13 +2796,13 @@
       <c r="D110" t="inlineStr"/>
       <c r="E110" t="inlineStr"/>
       <c r="F110" t="n">
-        <v>83002</v>
+        <v>83040</v>
       </c>
       <c r="G110" t="n">
         <v>109</v>
       </c>
       <c r="H110" t="n">
-        <v>0.3446998484187795</v>
+        <v>0.2478961367727529</v>
       </c>
     </row>
     <row r="111">
@@ -2818,13 +2818,13 @@
       <c r="D111" t="inlineStr"/>
       <c r="E111" t="inlineStr"/>
       <c r="F111" t="n">
-        <v>86981</v>
+        <v>87034</v>
       </c>
       <c r="G111" t="n">
         <v>110</v>
       </c>
       <c r="H111" t="n">
-        <v>0.3612242779127474</v>
+        <v>0.2598192722528875</v>
       </c>
     </row>
     <row r="112">
@@ -2840,13 +2840,13 @@
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="inlineStr"/>
       <c r="F112" t="n">
-        <v>90432</v>
+        <v>90507</v>
       </c>
       <c r="G112" t="n">
         <v>111</v>
       </c>
       <c r="H112" t="n">
-        <v>0.3755559708465707</v>
+        <v>0.270187086354667</v>
       </c>
     </row>
     <row r="113">
@@ -2862,13 +2862,13 @@
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="inlineStr"/>
       <c r="F113" t="n">
-        <v>93035</v>
+        <v>93112</v>
       </c>
       <c r="G113" t="n">
         <v>112</v>
       </c>
       <c r="H113" t="n">
-        <v>0.3863659959716771</v>
+        <v>0.2779636932464423</v>
       </c>
     </row>
     <row r="114">
@@ -2884,13 +2884,13 @@
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="inlineStr"/>
       <c r="F114" t="n">
-        <v>95965</v>
+        <v>96047</v>
       </c>
       <c r="G114" t="n">
         <v>113</v>
       </c>
       <c r="H114" t="n">
-        <v>0.3985340227164185</v>
+        <v>0.2867254365199012</v>
       </c>
     </row>
     <row r="115">
@@ -2906,13 +2906,13 @@
       <c r="D115" t="inlineStr"/>
       <c r="E115" t="inlineStr"/>
       <c r="F115" t="n">
-        <v>100990</v>
+        <v>101081</v>
       </c>
       <c r="G115" t="n">
         <v>114</v>
       </c>
       <c r="H115" t="n">
-        <v>0.4194023962291576</v>
+        <v>0.3017532442332206</v>
       </c>
     </row>
     <row r="116">
@@ -2928,13 +2928,13 @@
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="inlineStr"/>
       <c r="F116" t="n">
-        <v>106034</v>
+        <v>106138</v>
       </c>
       <c r="G116" t="n">
         <v>115</v>
       </c>
       <c r="H116" t="n">
-        <v>0.4403496750347806</v>
+        <v>0.3168497129670815</v>
       </c>
     </row>
     <row r="117">
@@ -2950,13 +2950,13 @@
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="inlineStr"/>
       <c r="F117" t="n">
-        <v>111184</v>
+        <v>111297</v>
       </c>
       <c r="G117" t="n">
         <v>116</v>
       </c>
       <c r="H117" t="n">
-        <v>0.4617371623164933</v>
+        <v>0.3322506784007356</v>
       </c>
     </row>
     <row r="118">
@@ -2972,13 +2972,13 @@
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="inlineStr"/>
       <c r="F118" t="n">
-        <v>116660</v>
+        <v>116876</v>
       </c>
       <c r="G118" t="n">
         <v>117</v>
       </c>
       <c r="H118" t="n">
-        <v>0.4844784983076891</v>
+        <v>0.3489054537747142</v>
       </c>
     </row>
     <row r="119">
@@ -2994,13 +2994,13 @@
       <c r="D119" t="inlineStr"/>
       <c r="E119" t="inlineStr"/>
       <c r="F119" t="n">
-        <v>121140</v>
+        <v>121522</v>
       </c>
       <c r="G119" t="n">
         <v>118</v>
       </c>
       <c r="H119" t="n">
-        <v>0.5030835357877033</v>
+        <v>0.3627749799241147</v>
       </c>
     </row>
     <row r="120">
@@ -3016,13 +3016,13 @@
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="inlineStr"/>
       <c r="F120" t="n">
-        <v>124687</v>
+        <v>125077</v>
       </c>
       <c r="G120" t="n">
         <v>119</v>
       </c>
       <c r="H120" t="n">
-        <v>0.5178139080960983</v>
+        <v>0.3733875854904337</v>
       </c>
     </row>
     <row r="121">
@@ -3038,13 +3038,13 @@
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="inlineStr"/>
       <c r="F121" t="n">
-        <v>128471</v>
+        <v>128881</v>
       </c>
       <c r="G121" t="n">
         <v>120</v>
       </c>
       <c r="H121" t="n">
-        <v>0.5335285201104674</v>
+        <v>0.3847435212356595</v>
       </c>
     </row>
     <row r="122">
@@ -3060,13 +3060,13 @@
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="inlineStr"/>
       <c r="F122" t="n">
-        <v>134372</v>
+        <v>134869</v>
       </c>
       <c r="G122" t="n">
         <v>121</v>
       </c>
       <c r="H122" t="n">
-        <v>0.5580348429161736</v>
+        <v>0.4026192686705734</v>
       </c>
     </row>
     <row r="123">
@@ -3082,13 +3082,13 @@
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="inlineStr"/>
       <c r="F123" t="n">
-        <v>140513</v>
+        <v>141081</v>
       </c>
       <c r="G123" t="n">
         <v>122</v>
       </c>
       <c r="H123" t="n">
-        <v>0.5835378641583089</v>
+        <v>0.421163714740327</v>
       </c>
     </row>
     <row r="124">
@@ -3104,13 +3104,13 @@
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="inlineStr"/>
       <c r="F124" t="n">
-        <v>146562</v>
+        <v>147286</v>
       </c>
       <c r="G124" t="n">
         <v>123</v>
       </c>
       <c r="H124" t="n">
-        <v>0.6086588176664798</v>
+        <v>0.4396872639777419</v>
       </c>
     </row>
     <row r="125">
@@ -3126,13 +3126,13 @@
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="inlineStr"/>
       <c r="F125" t="n">
-        <v>153194</v>
+        <v>154056</v>
       </c>
       <c r="G125" t="n">
         <v>124</v>
       </c>
       <c r="H125" t="n">
-        <v>0.6362009177931436</v>
+        <v>0.4598974861110697</v>
       </c>
     </row>
     <row r="126">
@@ -3148,13 +3148,13 @@
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="inlineStr"/>
       <c r="F126" t="n">
-        <v>159234</v>
+        <v>160284</v>
       </c>
       <c r="G126" t="n">
         <v>125</v>
       </c>
       <c r="H126" t="n">
-        <v>0.6612844951099482</v>
+        <v>0.4784896963690261</v>
       </c>
     </row>
     <row r="127">
@@ -3170,13 +3170,13 @@
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="inlineStr"/>
       <c r="F127" t="n">
-        <v>163526</v>
+        <v>164819</v>
       </c>
       <c r="G127" t="n">
         <v>126</v>
       </c>
       <c r="H127" t="n">
-        <v>0.6791087854814261</v>
+        <v>0.4920278584627693</v>
       </c>
     </row>
     <row r="128">
@@ -3192,13 +3192,13 @@
       <c r="D128" t="inlineStr"/>
       <c r="E128" t="inlineStr"/>
       <c r="F128" t="n">
-        <v>170138</v>
+        <v>172054</v>
       </c>
       <c r="G128" t="n">
         <v>127</v>
       </c>
       <c r="H128" t="n">
-        <v>0.7065678274050541</v>
+        <v>0.5136262273157421</v>
       </c>
     </row>
     <row r="129">
@@ -3214,13 +3214,13 @@
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="inlineStr"/>
       <c r="F129" t="n">
-        <v>176471</v>
+        <v>179003</v>
       </c>
       <c r="G129" t="n">
         <v>128</v>
       </c>
       <c r="H129" t="n">
-        <v>0.732868207396333</v>
+        <v>0.5343708113045892</v>
       </c>
     </row>
     <row r="130">
@@ -3236,13 +3236,13 @@
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="inlineStr"/>
       <c r="F130" t="n">
-        <v>183401</v>
+        <v>186734</v>
       </c>
       <c r="G130" t="n">
         <v>129</v>
       </c>
       <c r="H130" t="n">
-        <v>0.7616478747482298</v>
+        <v>0.5574498699918502</v>
       </c>
     </row>
     <row r="131">
@@ -3258,13 +3258,13 @@
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="inlineStr"/>
       <c r="F131" t="n">
-        <v>189220</v>
+        <v>193592</v>
       </c>
       <c r="G131" t="n">
         <v>130</v>
       </c>
       <c r="H131" t="n">
-        <v>0.7858136589214892</v>
+        <v>0.5779227951602937</v>
       </c>
     </row>
     <row r="132">
@@ -3280,13 +3280,13 @@
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="inlineStr"/>
       <c r="F132" t="n">
-        <v>195683</v>
+        <v>201362</v>
       </c>
       <c r="G132" t="n">
         <v>131</v>
       </c>
       <c r="H132" t="n">
-        <v>0.8126539172325007</v>
+        <v>0.601118279056299</v>
       </c>
     </row>
     <row r="133">
@@ -3302,13 +3302,13 @@
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="inlineStr"/>
       <c r="F133" t="n">
-        <v>200247</v>
+        <v>207620</v>
       </c>
       <c r="G133" t="n">
         <v>132</v>
       </c>
       <c r="H133" t="n">
-        <v>0.8316077991652651</v>
+        <v>0.6198000471671359</v>
       </c>
     </row>
     <row r="134">
@@ -3324,13 +3324,13 @@
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="inlineStr"/>
       <c r="F134" t="n">
-        <v>203478</v>
+        <v>212489</v>
       </c>
       <c r="G134" t="n">
         <v>133</v>
       </c>
       <c r="H134" t="n">
-        <v>0.8450258518656949</v>
+        <v>0.6343352866896134</v>
       </c>
     </row>
     <row r="135">
@@ -3346,13 +3346,13 @@
       <c r="D135" t="inlineStr"/>
       <c r="E135" t="inlineStr"/>
       <c r="F135" t="n">
-        <v>209190</v>
+        <v>221333</v>
       </c>
       <c r="G135" t="n">
         <v>134</v>
       </c>
       <c r="H135" t="n">
-        <v>0.8687472746527128</v>
+        <v>0.6607369417187346</v>
       </c>
     </row>
     <row r="136">
@@ -3368,13 +3368,13 @@
       <c r="D136" t="inlineStr"/>
       <c r="E136" t="inlineStr"/>
       <c r="F136" t="n">
-        <v>214849</v>
+        <v>229794</v>
       </c>
       <c r="G136" t="n">
         <v>135</v>
       </c>
       <c r="H136" t="n">
-        <v>0.892248593201686</v>
+        <v>0.6859952414927503</v>
       </c>
     </row>
     <row r="137">
@@ -3390,13 +3390,13 @@
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="inlineStr"/>
       <c r="F137" t="n">
-        <v>220115</v>
+        <v>237965</v>
       </c>
       <c r="G137" t="n">
         <v>136</v>
       </c>
       <c r="H137" t="n">
-        <v>0.9141178180610062</v>
+        <v>0.7103878153555895</v>
       </c>
     </row>
     <row r="138">
@@ -3412,13 +3412,13 @@
       <c r="D138" t="inlineStr"/>
       <c r="E138" t="inlineStr"/>
       <c r="F138" t="n">
-        <v>224696</v>
+        <v>246538</v>
       </c>
       <c r="G138" t="n">
         <v>137</v>
       </c>
       <c r="H138" t="n">
-        <v>0.9331422994663511</v>
+        <v>0.735980464447025</v>
       </c>
     </row>
     <row r="139">
@@ -3434,13 +3434,13 @@
       <c r="D139" t="inlineStr"/>
       <c r="E139" t="inlineStr"/>
       <c r="F139" t="n">
-        <v>228830</v>
+        <v>255205</v>
       </c>
       <c r="G139" t="n">
         <v>138</v>
       </c>
       <c r="H139" t="n">
-        <v>0.9503104300338462</v>
+        <v>0.7618537281441523</v>
       </c>
     </row>
     <row r="140">
@@ -3456,13 +3456,13 @@
       <c r="D140" t="inlineStr"/>
       <c r="E140" t="inlineStr"/>
       <c r="F140" t="n">
-        <v>231533</v>
+        <v>263677</v>
       </c>
       <c r="G140" t="n">
         <v>139</v>
       </c>
       <c r="H140" t="n">
-        <v>0.9615357461741315</v>
+        <v>0.7871448657975575</v>
       </c>
     </row>
     <row r="141">
@@ -3478,13 +3478,13 @@
       <c r="D141" t="inlineStr"/>
       <c r="E141" t="inlineStr"/>
       <c r="F141" t="n">
-        <v>233542</v>
+        <v>269196</v>
       </c>
       <c r="G141" t="n">
         <v>140</v>
       </c>
       <c r="H141" t="n">
-        <v>0.9698789426690754</v>
+        <v>0.8036205254657754</v>
       </c>
     </row>
     <row r="142">
@@ -3500,13 +3500,13 @@
       <c r="D142" t="inlineStr"/>
       <c r="E142" t="inlineStr"/>
       <c r="F142" t="n">
-        <v>235408</v>
+        <v>275270</v>
       </c>
       <c r="G142" t="n">
         <v>141</v>
       </c>
       <c r="H142" t="n">
-        <v>0.9776282730123134</v>
+        <v>0.8217530054122796</v>
       </c>
     </row>
     <row r="143">
@@ -3522,13 +3522,13 @@
       <c r="D143" t="inlineStr"/>
       <c r="E143" t="inlineStr"/>
       <c r="F143" t="n">
-        <v>237818</v>
+        <v>283953</v>
       </c>
       <c r="G143" t="n">
         <v>142</v>
       </c>
       <c r="H143" t="n">
-        <v>0.9876367864781246</v>
+        <v>0.8476740332976097</v>
       </c>
     </row>
     <row r="144">
@@ -3544,13 +3544,13 @@
       <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr"/>
       <c r="F144" t="n">
-        <v>239648</v>
+        <v>291622</v>
       </c>
       <c r="G144" t="n">
         <v>143</v>
       </c>
       <c r="H144" t="n">
-        <v>0.9952366120558982</v>
+        <v>0.8705680057555847</v>
       </c>
     </row>
     <row r="145">
@@ -3566,13 +3566,13 @@
       <c r="D145" t="inlineStr"/>
       <c r="E145" t="inlineStr"/>
       <c r="F145" t="n">
-        <v>240367</v>
+        <v>298503</v>
       </c>
       <c r="G145" t="n">
         <v>144</v>
       </c>
       <c r="H145" t="n">
-        <v>0.9982225544550344</v>
+        <v>0.8911095919445696</v>
       </c>
     </row>
     <row r="146">
@@ -3588,13 +3588,13 @@
       <c r="D146" t="inlineStr"/>
       <c r="E146" t="inlineStr"/>
       <c r="F146" t="n">
-        <v>240777</v>
+        <v>305304</v>
       </c>
       <c r="G146" t="n">
         <v>145</v>
       </c>
       <c r="H146" t="n">
-        <v>0.9999252476172678</v>
+        <v>0.9114123571925404</v>
       </c>
     </row>
     <row r="147">
@@ -3610,13 +3610,13 @@
       <c r="D147" t="inlineStr"/>
       <c r="E147" t="inlineStr"/>
       <c r="F147" t="n">
-        <v>240795</v>
+        <v>310220</v>
       </c>
       <c r="G147" t="n">
         <v>146</v>
       </c>
       <c r="H147" t="n">
-        <v>1</v>
+        <v>0.9260879040178638</v>
       </c>
     </row>
     <row r="148">
@@ -3627,17 +3627,223 @@
         <v>44038</v>
       </c>
       <c r="C148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr"/>
       <c r="F148" t="n">
-        <v>240795</v>
+        <v>313349</v>
       </c>
       <c r="G148" t="n">
         <v>147</v>
       </c>
       <c r="H148" t="n">
+        <v>0.9354287880732822</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" s="2" t="n">
+        <v>44039</v>
+      </c>
+      <c r="C149" t="n">
+        <v>1</v>
+      </c>
+      <c r="D149" t="inlineStr"/>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="n">
+        <v>319012</v>
+      </c>
+      <c r="G149" t="n">
+        <v>148</v>
+      </c>
+      <c r="H149" t="n">
+        <v>0.9523343254353258</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" s="2" t="n">
+        <v>44040</v>
+      </c>
+      <c r="C150" t="n">
+        <v>1</v>
+      </c>
+      <c r="D150" t="inlineStr"/>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="n">
+        <v>323648</v>
+      </c>
+      <c r="G150" t="n">
+        <v>149</v>
+      </c>
+      <c r="H150" t="n">
+        <v>0.9661739989670994</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" s="2" t="n">
+        <v>44041</v>
+      </c>
+      <c r="C151" t="n">
+        <v>1</v>
+      </c>
+      <c r="D151" t="inlineStr"/>
+      <c r="E151" t="inlineStr"/>
+      <c r="F151" t="n">
+        <v>327502</v>
+      </c>
+      <c r="G151" t="n">
+        <v>150</v>
+      </c>
+      <c r="H151" t="n">
+        <v>0.9776791978004591</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" s="2" t="n">
+        <v>44042</v>
+      </c>
+      <c r="C152" t="n">
+        <v>1</v>
+      </c>
+      <c r="D152" t="inlineStr"/>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="n">
+        <v>330722</v>
+      </c>
+      <c r="G152" t="n">
+        <v>151</v>
+      </c>
+      <c r="H152" t="n">
+        <v>0.9872917406762812</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" s="2" t="n">
+        <v>44043</v>
+      </c>
+      <c r="C153" t="n">
+        <v>1</v>
+      </c>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="n">
+        <v>332941</v>
+      </c>
+      <c r="G153" t="n">
+        <v>152</v>
+      </c>
+      <c r="H153" t="n">
+        <v>0.9939160365276629</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" s="2" t="n">
+        <v>44044</v>
+      </c>
+      <c r="C154" t="n">
+        <v>1</v>
+      </c>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr"/>
+      <c r="F154" t="n">
+        <v>334191</v>
+      </c>
+      <c r="G154" t="n">
+        <v>153</v>
+      </c>
+      <c r="H154" t="n">
+        <v>0.99764761373101</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" s="2" t="n">
+        <v>44045</v>
+      </c>
+      <c r="C155" t="n">
+        <v>1</v>
+      </c>
+      <c r="D155" t="inlineStr"/>
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="n">
+        <v>334596</v>
+      </c>
+      <c r="G155" t="n">
+        <v>154</v>
+      </c>
+      <c r="H155" t="n">
+        <v>0.9988566447448944</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" s="2" t="n">
+        <v>44046</v>
+      </c>
+      <c r="C156" t="n">
+        <v>1</v>
+      </c>
+      <c r="D156" t="inlineStr"/>
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="n">
+        <v>334962</v>
+      </c>
+      <c r="G156" t="n">
+        <v>155</v>
+      </c>
+      <c r="H156" t="n">
+        <v>0.9999492505500345</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" s="2" t="n">
+        <v>44047</v>
+      </c>
+      <c r="C157" t="n">
+        <v>1</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Valle de San José</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Santander</t>
+        </is>
+      </c>
+      <c r="F157" t="n">
+        <v>334979</v>
+      </c>
+      <c r="G157" t="n">
+        <v>156</v>
+      </c>
+      <c r="H157" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>